<commit_message>
support page dropdown menu
</commit_message>
<xml_diff>
--- a/data/SupportPageData.xlsx
+++ b/data/SupportPageData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashrafmahmoud/Documents/ITI/9 Months/Core courses/Data Visualization/Project/Story-of-Palestine-Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D8FA6A-E387-4F40-9EBA-30E66E35EA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{666264C8-DD7B-FC40-BE27-DE07E7F99F63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DA82F47E-9593-7045-8AD3-0C2B15578C02}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>organization</t>
   </si>
@@ -101,18 +101,6 @@
     <t>https://www.wfp.org/</t>
   </si>
   <si>
-    <t>International Committee of the Red Cross</t>
-  </si>
-  <si>
-    <t>The ICRC operates worldwide, helping people affected by conflict and armed violence and promoting the laws that protect victims of war.</t>
-  </si>
-  <si>
-    <t>https://www.icrc.org/en/donate/gaza-is-powerless</t>
-  </si>
-  <si>
-    <t>https://www.icrc.org/</t>
-  </si>
-  <si>
     <t>Zakat Foundation of America</t>
   </si>
   <si>
@@ -195,51 +183,6 @@
   </si>
   <si>
     <t>https://www.krcs.org.kw/</t>
-  </si>
-  <si>
-    <t>Call For a Ceasefire</t>
-  </si>
-  <si>
-    <t>Call and Email your representative in the congress and demand a ceasefire. Lives can be saved in Gaza just by putting enough pressure on Politicians that in turn put pressure on Israel to stop this massacre.</t>
-  </si>
-  <si>
-    <t>https://act.uscpr.org/a/callforgaza</t>
-  </si>
-  <si>
-    <t>Go To Protests</t>
-  </si>
-  <si>
-    <t>Expressing solidarity with Palestine through participation in protests, marches, rallies, and vigils encourages both ordinary citizens and policymakers to give greater attention and gravity to the ongoing massacre.</t>
-  </si>
-  <si>
-    <t>https://uscpr.org/oct-2023-protests/</t>
-  </si>
-  <si>
-    <t>Spread The Word</t>
-  </si>
-  <si>
-    <t>Amplify the voices of those shining a light on the human rights abuses being committed by the IDF against the people of Gaza; otherwise, no one will know anything to stop them. Don't hesitate to share this website and engage in debates to make clear of the truth.</t>
-  </si>
-  <si>
-    <t>https://twitter.com/intent/tweet?url=${link}&amp;text=${text}</t>
-  </si>
-  <si>
-    <t>Boycott</t>
-  </si>
-  <si>
-    <t>You could contribute in restoring peace to Palestine by pressuring Israel to comply with international humanitarian law by boycotting products that support the ongoing genocide.</t>
-  </si>
-  <si>
-    <t>https://boycott.thewitness.news/</t>
-  </si>
-  <si>
-    <t>Pray</t>
-  </si>
-  <si>
-    <t>Pray for those starving, suffering and dying in Gaza. Pray that peace could be bestowed upon their land once again and that they could be brought back to their homes safely.</t>
-  </si>
-  <si>
-    <t>https://www.islamic-relief.org.uk/giving/appeals/palestine/pray-for-palestine/#:~:text=O%20Allah%2C%20help%20and%20protect,in%20this%20time%20of%20crisis.</t>
   </si>
   <si>
     <t>"./SupportPage/Unicef-logo.jpeg",
@@ -264,10 +207,6 @@
             "./SupportPage/WFP-3.jpg",</t>
   </si>
   <si>
-    <t>"./SupportPage/RedCrossLogo.png",
-            "./SupportPage/ICRC-1.jpg",</t>
-  </si>
-  <si>
     <t>"./SupportPage/prc-logo.png",
             "./SupportPage/prc.png",</t>
   </si>
@@ -303,21 +242,6 @@
             "./SupportPage/ZFA-2.jpg",</t>
   </si>
   <si>
-    <t>./SupportPage/congress-better.webp</t>
-  </si>
-  <si>
-    <t>"./HomePage/paly.jpeg"</t>
-  </si>
-  <si>
-    <t>./SupportPage/hamas.jpeg</t>
-  </si>
-  <si>
-    <t>./SupportPage/pray.jpeg</t>
-  </si>
-  <si>
-    <t>./SupportPage/boycott.jpeg</t>
-  </si>
-  <si>
     <t>UnicefLogo.png</t>
   </si>
   <si>
@@ -325,9 +249,6 @@
   </si>
   <si>
     <t>WorldFoodProgrammeLogo.png</t>
-  </si>
-  <si>
-    <t>RedCrossLogo.png</t>
   </si>
   <si>
     <t>ZakatFoundationLogo.png</t>
@@ -352,7 +273,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -367,11 +288,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -395,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,9 +320,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,21 +657,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5978B93A-5D86-9C4F-93AD-00311E57D08A}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="88" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="213.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="139.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="222.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="91.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="143.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -782,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -802,10 +714,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -825,10 +737,10 @@
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -848,13 +760,13 @@
         <v>20</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -868,13 +780,13 @@
         <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -888,189 +800,99 @@
         <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>72</v>
+      <c r="F8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1081,25 +903,18 @@
     <hyperlink ref="E3" r:id="rId4" xr:uid="{8600EE1D-59F0-D340-887E-12A0E8832F15}"/>
     <hyperlink ref="D4" r:id="rId5" xr:uid="{B80A282B-C2A6-BB4C-ACC8-C537C4719A25}"/>
     <hyperlink ref="E4" r:id="rId6" xr:uid="{48F56399-9005-074B-A20E-7F9A335A1538}"/>
-    <hyperlink ref="D5" r:id="rId7" xr:uid="{57A2EFA3-E9C6-EB4B-A2B2-A087484793F1}"/>
-    <hyperlink ref="E5" r:id="rId8" xr:uid="{1CE6EF06-B6EB-AC42-B1D6-59C1DE92B705}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{C5BFFCC8-CA22-8F43-B758-4F5AF410F26E}"/>
-    <hyperlink ref="E6" r:id="rId10" xr:uid="{FE6E65C0-BE3B-0949-A58D-364341E9ADCD}"/>
-    <hyperlink ref="D7" r:id="rId11" xr:uid="{92BC4F12-C6D1-A34E-A4EB-7CA42C076159}"/>
-    <hyperlink ref="E7" r:id="rId12" xr:uid="{B2EDDC48-2E18-444B-972C-E9004144E72B}"/>
-    <hyperlink ref="D9" r:id="rId13" xr:uid="{18667951-D886-D44F-8C56-328918FC7F80}"/>
-    <hyperlink ref="E9" r:id="rId14" xr:uid="{7723300E-D686-C949-8539-D3028A45B1A9}"/>
-    <hyperlink ref="D10" r:id="rId15" xr:uid="{31AFB4FA-B168-534C-A31F-D273B366FD19}"/>
-    <hyperlink ref="E10" r:id="rId16" xr:uid="{B318D30D-5611-B145-B008-0D152E8CF7A9}"/>
-    <hyperlink ref="D11" r:id="rId17" xr:uid="{B19C561F-DBD0-ED49-B4BB-D92723BC640B}"/>
-    <hyperlink ref="E11" r:id="rId18" xr:uid="{27770B3C-EB48-8943-AD7B-0F20F492B3A8}"/>
-    <hyperlink ref="D8" r:id="rId19" xr:uid="{765FC0BB-1C3E-C34C-97A0-160D2890A12C}"/>
-    <hyperlink ref="E8" r:id="rId20" xr:uid="{7056CE25-3AEA-6049-8DF1-0E2DC86D4EA9}"/>
-    <hyperlink ref="E12" r:id="rId21" xr:uid="{F76A1522-90AC-F94C-9D5E-D3067A4C2C91}"/>
-    <hyperlink ref="E13" r:id="rId22" xr:uid="{16F30E42-9423-6C44-9822-2FF35FD5831B}"/>
-    <hyperlink ref="E14" r:id="rId23" xr:uid="{7F1F4394-9AAF-7049-AAD9-290083FE0353}"/>
-    <hyperlink ref="E15" r:id="rId24" xr:uid="{2A4E9945-A1D9-F348-B07A-24631EE004BB}"/>
-    <hyperlink ref="E16" r:id="rId25" location=":~:text=O%20Allah%2C%20help%20and%20protect,in%20this%20time%20of%20crisis." xr:uid="{0580BE17-FFFD-3B4E-854D-33A19E46E4EC}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{C5BFFCC8-CA22-8F43-B758-4F5AF410F26E}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{FE6E65C0-BE3B-0949-A58D-364341E9ADCD}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{92BC4F12-C6D1-A34E-A4EB-7CA42C076159}"/>
+    <hyperlink ref="E6" r:id="rId10" xr:uid="{B2EDDC48-2E18-444B-972C-E9004144E72B}"/>
+    <hyperlink ref="D8" r:id="rId11" xr:uid="{18667951-D886-D44F-8C56-328918FC7F80}"/>
+    <hyperlink ref="E8" r:id="rId12" xr:uid="{7723300E-D686-C949-8539-D3028A45B1A9}"/>
+    <hyperlink ref="D9" r:id="rId13" xr:uid="{31AFB4FA-B168-534C-A31F-D273B366FD19}"/>
+    <hyperlink ref="E9" r:id="rId14" xr:uid="{B318D30D-5611-B145-B008-0D152E8CF7A9}"/>
+    <hyperlink ref="D10" r:id="rId15" xr:uid="{B19C561F-DBD0-ED49-B4BB-D92723BC640B}"/>
+    <hyperlink ref="E10" r:id="rId16" xr:uid="{27770B3C-EB48-8943-AD7B-0F20F492B3A8}"/>
+    <hyperlink ref="D7" r:id="rId17" xr:uid="{765FC0BB-1C3E-C34C-97A0-160D2890A12C}"/>
+    <hyperlink ref="E7" r:id="rId18" xr:uid="{7056CE25-3AEA-6049-8DF1-0E2DC86D4EA9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>